<commit_message>
update reference files (make sure to use the correct 12.5 fg/cell for pro
</commit_message>
<xml_diff>
--- a/STORE_model/reference_10cc_axenic.xlsx
+++ b/STORE_model/reference_10cc_axenic.xlsx
@@ -554,10 +554,10 @@
         <v>0.034</v>
       </c>
       <c r="L3">
-        <v>0.7973095922961667</v>
+        <v>0.7973095922961668</v>
       </c>
       <c r="M3">
-        <v>5.282176048962104</v>
+        <v>5.282176048962105</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -595,10 +595,10 @@
         <v>0.159</v>
       </c>
       <c r="L4">
-        <v>3.728594858090897</v>
+        <v>3.728594858090898</v>
       </c>
       <c r="M4">
-        <v>24.70194093485219</v>
+        <v>24.7019409348522</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -677,7 +677,7 @@
         <v>0.306</v>
       </c>
       <c r="L6">
-        <v>7.175786330665499</v>
+        <v>7.1757863306655</v>
       </c>
       <c r="M6">
         <v>47.53958444065893</v>
@@ -721,7 +721,7 @@
         <v>12.42864952696966</v>
       </c>
       <c r="M7">
-        <v>82.33980311617397</v>
+        <v>82.339803116174</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -759,10 +759,10 @@
         <v>1.026</v>
       </c>
       <c r="L8">
-        <v>24.05998946164314</v>
+        <v>24.05998946164315</v>
       </c>
       <c r="M8">
-        <v>159.3974301833858</v>
+        <v>159.3974301833859</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -841,10 +841,10 @@
         <v>2.699</v>
       </c>
       <c r="L10">
-        <v>63.29231145903981</v>
+        <v>63.29231145903982</v>
       </c>
       <c r="M10">
-        <v>419.3115634161387</v>
+        <v>419.3115634161388</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -882,10 +882,10 @@
         <v>2.415</v>
       </c>
       <c r="L11">
-        <v>56.63243133515419</v>
+        <v>56.6324313351542</v>
       </c>
       <c r="M11">
-        <v>375.1898575953965</v>
+        <v>375.1898575953966</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1128,7 +1128,7 @@
         <v>0.725</v>
       </c>
       <c r="L17">
-        <v>17.00145454160943</v>
+        <v>17.00145454160944</v>
       </c>
       <c r="M17">
         <v>112.6346363381625</v>
@@ -1169,7 +1169,7 @@
         <v>0.6906666666666667</v>
       </c>
       <c r="L18">
-        <v>16.19632818860448</v>
+        <v>16.19632818860449</v>
       </c>
       <c r="M18">
         <v>107.3006742495047</v>
@@ -1213,7 +1213,7 @@
         <v>13.32757700848004</v>
       </c>
       <c r="M19">
-        <v>88.29519768118026</v>
+        <v>88.29519768118028</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1292,10 +1292,10 @@
         <v>0.407</v>
       </c>
       <c r="L21">
-        <v>9.544264825427641</v>
+        <v>9.544264825427643</v>
       </c>
       <c r="M21">
-        <v>63.23075446845812</v>
+        <v>63.23075446845814</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -1377,7 +1377,7 @@
         <v>6.894382945149206</v>
       </c>
       <c r="M23">
-        <v>45.67528701161348</v>
+        <v>45.6752870116135</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1456,7 +1456,7 @@
         <v>0.2163333333333333</v>
       </c>
       <c r="L25">
-        <v>5.07307770000208</v>
+        <v>5.073077700002081</v>
       </c>
       <c r="M25">
         <v>33.60913976251378</v>
@@ -1538,7 +1538,7 @@
         <v>0.107</v>
       </c>
       <c r="L27">
-        <v>2.509180187520289</v>
+        <v>2.50918018752029</v>
       </c>
       <c r="M27">
         <v>16.62331874232192</v>
@@ -1582,7 +1582,7 @@
         <v>0.04690056425271569</v>
       </c>
       <c r="M28">
-        <v>0.3107162381742414</v>
+        <v>0.3107162381742415</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -1620,10 +1620,10 @@
         <v>-0.032</v>
       </c>
       <c r="L29">
-        <v>-0.750409028043451</v>
+        <v>-0.7504090280434511</v>
       </c>
       <c r="M29">
-        <v>-4.971459810787863</v>
+        <v>-4.971459810787864</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -1664,7 +1664,7 @@
         <v>1.078712977812461</v>
       </c>
       <c r="M30">
-        <v>7.146473478007553</v>
+        <v>7.146473478007554</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -1702,10 +1702,10 @@
         <v>0.03533333333333333</v>
       </c>
       <c r="L31">
-        <v>0.8285766351313103</v>
+        <v>0.8285766351313105</v>
       </c>
       <c r="M31">
-        <v>5.489320207744932</v>
+        <v>5.489320207744933</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -1743,10 +1743,10 @@
         <v>0.03533333333333333</v>
       </c>
       <c r="L32">
-        <v>0.8285766351313105</v>
+        <v>0.8285766351313106</v>
       </c>
       <c r="M32">
-        <v>5.489320207744932</v>
+        <v>5.489320207744933</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -1784,7 +1784,7 @@
         <v>0.03</v>
       </c>
       <c r="L33">
-        <v>0.7035084637907353</v>
+        <v>0.7035084637907354</v>
       </c>
       <c r="M33">
         <v>4.660743572613621</v>
@@ -1825,10 +1825,10 @@
         <v>-0.038</v>
       </c>
       <c r="L34">
-        <v>-0.8911107208015979</v>
+        <v>-0.891110720801598</v>
       </c>
       <c r="M34">
-        <v>-5.903608525310586</v>
+        <v>-5.903608525310587</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -1866,10 +1866,10 @@
         <v>0.04666666666666667</v>
       </c>
       <c r="L35">
-        <v>1.094346499230032</v>
+        <v>1.094346499230033</v>
       </c>
       <c r="M35">
-        <v>7.250045557398966</v>
+        <v>7.250045557398967</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -1907,10 +1907,10 @@
         <v>0.03933333333333334</v>
       </c>
       <c r="L36">
-        <v>0.9223777636367417</v>
+        <v>0.922377763636742</v>
       </c>
       <c r="M36">
-        <v>6.110752684093414</v>
+        <v>6.110752684093415</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -1951,7 +1951,7 @@
         <v>0.445555360400799</v>
       </c>
       <c r="M37">
-        <v>2.951804262655293</v>
+        <v>2.951804262655294</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -1989,10 +1989,10 @@
         <v>0.048</v>
       </c>
       <c r="L38">
-        <v>1.125613542065176</v>
+        <v>1.125613542065177</v>
       </c>
       <c r="M38">
-        <v>7.457189716181794</v>
+        <v>7.457189716181796</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -2074,7 +2074,7 @@
         <v>0.445555360400799</v>
       </c>
       <c r="M40">
-        <v>2.951804262655293</v>
+        <v>2.951804262655294</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -2156,7 +2156,7 @@
         <v>1.219414670570608</v>
       </c>
       <c r="M42">
-        <v>8.078622192530275</v>
+        <v>8.078622192530277</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -2194,10 +2194,10 @@
         <v>0.033</v>
       </c>
       <c r="L43">
-        <v>0.7738593101698088</v>
+        <v>0.7738593101698089</v>
       </c>
       <c r="M43">
-        <v>5.126817929874983</v>
+        <v>5.126817929874984</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -2443,7 +2443,7 @@
         <v>0.445555360400799</v>
       </c>
       <c r="M49">
-        <v>2.951804262655293</v>
+        <v>2.951804262655294</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -2563,7 +2563,7 @@
         <v>0.039</v>
       </c>
       <c r="L52">
-        <v>0.9145610029279557</v>
+        <v>0.9145610029279558</v>
       </c>
       <c r="M52">
         <v>6.058966644397707</v>
@@ -2604,10 +2604,10 @@
         <v>0.024</v>
       </c>
       <c r="L53">
-        <v>0.5628067710325882</v>
+        <v>0.5628067710325884</v>
       </c>
       <c r="M53">
-        <v>3.728594858090897</v>
+        <v>3.728594858090898</v>
       </c>
     </row>
     <row r="54" spans="1:13">
@@ -2686,10 +2686,10 @@
         <v>0.024</v>
       </c>
       <c r="L55">
-        <v>0.5628067710325882</v>
+        <v>0.5628067710325884</v>
       </c>
       <c r="M55">
-        <v>3.728594858090897</v>
+        <v>3.728594858090898</v>
       </c>
     </row>
     <row r="56" spans="1:13">
@@ -2727,7 +2727,7 @@
         <v>0.029</v>
       </c>
       <c r="L56">
-        <v>0.6800581816643775</v>
+        <v>0.6800581816643776</v>
       </c>
       <c r="M56">
         <v>4.505385453526501</v>
@@ -2768,7 +2768,7 @@
         <v>0.028</v>
       </c>
       <c r="L57">
-        <v>0.6566078995380196</v>
+        <v>0.6566078995380197</v>
       </c>
       <c r="M57">
         <v>4.35002733443938</v>
@@ -2809,10 +2809,10 @@
         <v>0.034</v>
       </c>
       <c r="L58">
-        <v>0.7973095922961667</v>
+        <v>0.7973095922961668</v>
       </c>
       <c r="M58">
-        <v>5.282176048962104</v>
+        <v>5.282176048962105</v>
       </c>
     </row>
     <row r="59" spans="1:13">
@@ -2850,10 +2850,10 @@
         <v>0.048</v>
       </c>
       <c r="L59">
-        <v>1.125613542065176</v>
+        <v>1.125613542065177</v>
       </c>
       <c r="M59">
-        <v>7.457189716181794</v>
+        <v>7.457189716181796</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -2891,7 +2891,7 @@
         <v>0.029</v>
       </c>
       <c r="L60">
-        <v>0.6800581816643775</v>
+        <v>0.6800581816643776</v>
       </c>
       <c r="M60">
         <v>4.505385453526501</v>
@@ -3014,10 +3014,10 @@
         <v>0.024</v>
       </c>
       <c r="L63">
-        <v>0.5628067710325882</v>
+        <v>0.5628067710325884</v>
       </c>
       <c r="M63">
-        <v>3.728594858090897</v>
+        <v>3.728594858090898</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -3096,10 +3096,10 @@
         <v>0.048</v>
       </c>
       <c r="L65">
-        <v>1.125613542065176</v>
+        <v>1.125613542065177</v>
       </c>
       <c r="M65">
-        <v>7.457189716181794</v>
+        <v>7.457189716181796</v>
       </c>
     </row>
     <row r="66" spans="1:13">
@@ -3137,10 +3137,10 @@
         <v>-0.033</v>
       </c>
       <c r="L66">
-        <v>-0.7738593101698088</v>
+        <v>-0.7738593101698089</v>
       </c>
       <c r="M66">
-        <v>-5.126817929874983</v>
+        <v>-5.126817929874984</v>
       </c>
     </row>
     <row r="67" spans="1:13">
@@ -3178,10 +3178,10 @@
         <v>0.038</v>
       </c>
       <c r="L67">
-        <v>0.8911107208015979</v>
+        <v>0.891110720801598</v>
       </c>
       <c r="M67">
-        <v>5.903608525310586</v>
+        <v>5.903608525310587</v>
       </c>
     </row>
     <row r="68" spans="1:13">
@@ -3263,7 +3263,7 @@
         <v>0.445555360400799</v>
       </c>
       <c r="M69">
-        <v>2.951804262655293</v>
+        <v>2.951804262655294</v>
       </c>
     </row>
     <row r="70" spans="1:13">
@@ -3301,10 +3301,10 @@
         <v>0.033</v>
       </c>
       <c r="L70">
-        <v>0.7738593101698088</v>
+        <v>0.7738593101698089</v>
       </c>
       <c r="M70">
-        <v>5.126817929874983</v>
+        <v>5.126817929874984</v>
       </c>
     </row>
     <row r="71" spans="1:13">
@@ -3342,7 +3342,7 @@
         <v>0.029</v>
       </c>
       <c r="L71">
-        <v>0.6800581816643775</v>
+        <v>0.6800581816643776</v>
       </c>
       <c r="M71">
         <v>4.505385453526501</v>
@@ -3427,7 +3427,7 @@
         <v>1.219414670570608</v>
       </c>
       <c r="M73">
-        <v>8.078622192530275</v>
+        <v>8.078622192530277</v>
       </c>
     </row>
     <row r="74" spans="1:13">
@@ -3506,10 +3506,10 @@
         <v>0.033</v>
       </c>
       <c r="L75">
-        <v>0.7738593101698088</v>
+        <v>0.7738593101698089</v>
       </c>
       <c r="M75">
-        <v>5.126817929874983</v>
+        <v>5.126817929874984</v>
       </c>
     </row>
     <row r="76" spans="1:13">
@@ -3591,7 +3591,7 @@
         <v>1.453917491834186</v>
       </c>
       <c r="M77">
-        <v>9.632203383401484</v>
+        <v>9.632203383401485</v>
       </c>
     </row>
     <row r="78" spans="1:13">
@@ -3670,7 +3670,7 @@
         <v>0.228</v>
       </c>
       <c r="L79">
-        <v>5.346664324809588</v>
+        <v>5.346664324809589</v>
       </c>
       <c r="M79">
         <v>35.42165115186352</v>
@@ -3711,10 +3711,10 @@
         <v>0.327</v>
       </c>
       <c r="L80">
-        <v>7.668242255319014</v>
+        <v>7.668242255319016</v>
       </c>
       <c r="M80">
-        <v>50.80210494148847</v>
+        <v>50.80210494148848</v>
       </c>
     </row>
     <row r="81" spans="1:13">
@@ -3793,7 +3793,7 @@
         <v>0.981</v>
       </c>
       <c r="L82">
-        <v>23.00472676595704</v>
+        <v>23.00472676595705</v>
       </c>
       <c r="M82">
         <v>152.4063148244654</v>
@@ -3875,10 +3875,10 @@
         <v>2.9</v>
       </c>
       <c r="L84">
-        <v>68.00581816643773</v>
+        <v>68.00581816643775</v>
       </c>
       <c r="M84">
-        <v>450.53854535265</v>
+        <v>450.5385453526501</v>
       </c>
     </row>
     <row r="85" spans="1:13">
@@ -3916,10 +3916,10 @@
         <v>2.541</v>
       </c>
       <c r="L85">
-        <v>59.58716688307527</v>
+        <v>59.58716688307528</v>
       </c>
       <c r="M85">
-        <v>394.7649806003736</v>
+        <v>394.7649806003737</v>
       </c>
     </row>
     <row r="86" spans="1:13">
@@ -3957,7 +3957,7 @@
         <v>1.693666666666666</v>
       </c>
       <c r="L86">
-        <v>39.71696116134139</v>
+        <v>39.7169611613414</v>
       </c>
       <c r="M86">
         <v>263.1248676938868</v>
@@ -4039,7 +4039,7 @@
         <v>0.9976666666666666</v>
       </c>
       <c r="L88">
-        <v>23.39556480139634</v>
+        <v>23.39556480139635</v>
       </c>
       <c r="M88">
         <v>154.9956168092508</v>
@@ -4080,10 +4080,10 @@
         <v>0.8906666666666667</v>
       </c>
       <c r="L89">
-        <v>20.88638461387605</v>
+        <v>20.88638461387606</v>
       </c>
       <c r="M89">
-        <v>138.3722980669288</v>
+        <v>138.3722980669289</v>
       </c>
     </row>
     <row r="90" spans="1:13">
@@ -4121,7 +4121,7 @@
         <v>0.9373333333333335</v>
       </c>
       <c r="L90">
-        <v>21.98073111310608</v>
+        <v>21.98073111310609</v>
       </c>
       <c r="M90">
         <v>145.6223436243278</v>
@@ -4165,7 +4165,7 @@
         <v>14.60952576472094</v>
       </c>
       <c r="M91">
-        <v>96.78810819127619</v>
+        <v>96.78810819127621</v>
       </c>
     </row>
     <row r="92" spans="1:13">
@@ -4244,10 +4244,10 @@
         <v>0.522</v>
       </c>
       <c r="L93">
-        <v>12.24104726995879</v>
+        <v>12.2410472699588</v>
       </c>
       <c r="M93">
-        <v>81.09693816347702</v>
+        <v>81.09693816347703</v>
       </c>
     </row>
     <row r="94" spans="1:13">
@@ -4285,10 +4285,10 @@
         <v>0.3793333333333333</v>
       </c>
       <c r="L94">
-        <v>8.895473686598407</v>
+        <v>8.895473686598409</v>
       </c>
       <c r="M94">
-        <v>58.93251317371445</v>
+        <v>58.93251317371446</v>
       </c>
     </row>
     <row r="95" spans="1:13">
@@ -4367,10 +4367,10 @@
         <v>0.267</v>
       </c>
       <c r="L96">
-        <v>6.261225327737544</v>
+        <v>6.261225327737545</v>
       </c>
       <c r="M96">
-        <v>41.48061779626122</v>
+        <v>41.48061779626124</v>
       </c>
     </row>
     <row r="97" spans="1:13">
@@ -4408,7 +4408,7 @@
         <v>0.166</v>
       </c>
       <c r="L97">
-        <v>3.892746832975401</v>
+        <v>3.892746832975402</v>
       </c>
       <c r="M97">
         <v>25.78944776846204</v>
@@ -4449,7 +4449,7 @@
         <v>0.117</v>
       </c>
       <c r="L98">
-        <v>2.743683008783867</v>
+        <v>2.743683008783868</v>
       </c>
       <c r="M98">
         <v>18.17689993319312</v>
@@ -4572,10 +4572,10 @@
         <v>0.06133333333333333</v>
       </c>
       <c r="L101">
-        <v>1.438283970416614</v>
+        <v>1.438283970416615</v>
       </c>
       <c r="M101">
-        <v>9.528631304010069</v>
+        <v>9.528631304010071</v>
       </c>
     </row>
     <row r="102" spans="1:13">
@@ -4654,10 +4654,10 @@
         <v>-0.018</v>
       </c>
       <c r="L103">
-        <v>-0.4221050782744411</v>
+        <v>-0.4221050782744412</v>
       </c>
       <c r="M103">
-        <v>-2.796446143568172</v>
+        <v>-2.796446143568173</v>
       </c>
     </row>
     <row r="104" spans="1:13">
@@ -4736,10 +4736,10 @@
         <v>0.02733333333333333</v>
       </c>
       <c r="L105">
-        <v>0.6409743781204477</v>
+        <v>0.6409743781204479</v>
       </c>
       <c r="M105">
-        <v>4.246455255047966</v>
+        <v>4.246455255047967</v>
       </c>
     </row>
     <row r="106" spans="1:13">
@@ -4777,10 +4777,10 @@
         <v>0.04933333333333333</v>
       </c>
       <c r="L106">
-        <v>1.15688058490032</v>
+        <v>1.156880584900321</v>
       </c>
       <c r="M106">
-        <v>7.664333874964622</v>
+        <v>7.664333874964623</v>
       </c>
     </row>
     <row r="107" spans="1:13">
@@ -4821,7 +4821,7 @@
         <v>1.070896217103675</v>
       </c>
       <c r="M107">
-        <v>7.094687438311844</v>
+        <v>7.094687438311847</v>
       </c>
     </row>
     <row r="108" spans="1:13">
@@ -4859,7 +4859,7 @@
         <v>-0.015</v>
       </c>
       <c r="L108">
-        <v>-0.3517542318953676</v>
+        <v>-0.3517542318953677</v>
       </c>
       <c r="M108">
         <v>-2.330371786306811</v>
@@ -4941,7 +4941,7 @@
         <v>0.017</v>
       </c>
       <c r="L110">
-        <v>0.3986547961480833</v>
+        <v>0.3986547961480834</v>
       </c>
       <c r="M110">
         <v>2.641088024481052</v>
@@ -5026,7 +5026,7 @@
         <v>-0.445555360400799</v>
       </c>
       <c r="M112">
-        <v>-2.951804262655293</v>
+        <v>-2.951804262655294</v>
       </c>
     </row>
     <row r="113" spans="1:13">
@@ -5228,10 +5228,10 @@
         <v>0.024</v>
       </c>
       <c r="L117">
-        <v>0.5628067710325882</v>
+        <v>0.5628067710325884</v>
       </c>
       <c r="M117">
-        <v>3.728594858090897</v>
+        <v>3.728594858090898</v>
       </c>
     </row>
     <row r="118" spans="1:13">
@@ -5559,7 +5559,7 @@
         <v>0.445555360400799</v>
       </c>
       <c r="M125">
-        <v>2.951804262655293</v>
+        <v>2.951804262655294</v>
       </c>
     </row>
     <row r="126" spans="1:13">
@@ -5597,10 +5597,10 @@
         <v>0.034</v>
       </c>
       <c r="L126">
-        <v>0.7973095922961667</v>
+        <v>0.7973095922961668</v>
       </c>
       <c r="M126">
-        <v>5.282176048962104</v>
+        <v>5.282176048962105</v>
       </c>
     </row>
     <row r="127" spans="1:13">
@@ -5720,10 +5720,10 @@
         <v>0.024</v>
       </c>
       <c r="L129">
-        <v>0.5628067710325882</v>
+        <v>0.5628067710325884</v>
       </c>
       <c r="M129">
-        <v>3.728594858090897</v>
+        <v>3.728594858090898</v>
       </c>
     </row>
     <row r="130" spans="1:13">
@@ -5805,7 +5805,7 @@
         <v>0.445555360400799</v>
       </c>
       <c r="M131">
-        <v>2.951804262655293</v>
+        <v>2.951804262655294</v>
       </c>
     </row>
     <row r="132" spans="1:13">
@@ -5843,7 +5843,7 @@
         <v>0.015</v>
       </c>
       <c r="L132">
-        <v>0.3517542318953676</v>
+        <v>0.3517542318953677</v>
       </c>
       <c r="M132">
         <v>2.330371786306811</v>
@@ -5925,10 +5925,10 @@
         <v>0.024</v>
       </c>
       <c r="L134">
-        <v>0.5628067710325882</v>
+        <v>0.5628067710325884</v>
       </c>
       <c r="M134">
-        <v>3.728594858090897</v>
+        <v>3.728594858090898</v>
       </c>
     </row>
     <row r="135" spans="1:13">
@@ -5966,10 +5966,10 @@
         <v>0.033</v>
       </c>
       <c r="L135">
-        <v>0.7738593101698088</v>
+        <v>0.7738593101698089</v>
       </c>
       <c r="M135">
-        <v>5.126817929874983</v>
+        <v>5.126817929874984</v>
       </c>
     </row>
     <row r="136" spans="1:13">
@@ -6130,10 +6130,10 @@
         <v>0.024</v>
       </c>
       <c r="L139">
-        <v>0.5628067710325882</v>
+        <v>0.5628067710325884</v>
       </c>
       <c r="M139">
-        <v>3.728594858090897</v>
+        <v>3.728594858090898</v>
       </c>
     </row>
     <row r="140" spans="1:13">
@@ -6212,7 +6212,7 @@
         <v>0.028</v>
       </c>
       <c r="L141">
-        <v>0.6566078995380196</v>
+        <v>0.6566078995380197</v>
       </c>
       <c r="M141">
         <v>4.35002733443938</v>
@@ -6253,7 +6253,7 @@
         <v>0.029</v>
       </c>
       <c r="L142">
-        <v>0.6800581816643775</v>
+        <v>0.6800581816643776</v>
       </c>
       <c r="M142">
         <v>4.505385453526501</v>
@@ -6294,10 +6294,10 @@
         <v>0.038</v>
       </c>
       <c r="L143">
-        <v>0.8911107208015979</v>
+        <v>0.891110720801598</v>
       </c>
       <c r="M143">
-        <v>5.903608525310586</v>
+        <v>5.903608525310587</v>
       </c>
     </row>
     <row r="144" spans="1:13">
@@ -6461,7 +6461,7 @@
         <v>1.477367773960544</v>
       </c>
       <c r="M147">
-        <v>9.787561502488606</v>
+        <v>9.787561502488607</v>
       </c>
     </row>
     <row r="148" spans="1:13">
@@ -6499,7 +6499,7 @@
         <v>0.015</v>
       </c>
       <c r="L148">
-        <v>0.3517542318953676</v>
+        <v>0.3517542318953677</v>
       </c>
       <c r="M148">
         <v>2.330371786306811</v>
@@ -6543,7 +6543,7 @@
         <v>0.445555360400799</v>
       </c>
       <c r="M149">
-        <v>2.951804262655293</v>
+        <v>2.951804262655294</v>
       </c>
     </row>
     <row r="150" spans="1:13">
@@ -6581,10 +6581,10 @@
         <v>0.181</v>
       </c>
       <c r="L150">
-        <v>4.244501064870769</v>
+        <v>4.24450106487077</v>
       </c>
       <c r="M150">
-        <v>28.11981955476884</v>
+        <v>28.11981955476885</v>
       </c>
     </row>
     <row r="151" spans="1:13">
@@ -6625,7 +6625,7 @@
         <v>1.500818056086902</v>
       </c>
       <c r="M151">
-        <v>9.942919621575726</v>
+        <v>9.942919621575728</v>
       </c>
     </row>
     <row r="152" spans="1:13">
@@ -6663,7 +6663,7 @@
         <v>0.155</v>
       </c>
       <c r="L152">
-        <v>3.634793729585465</v>
+        <v>3.634793729585466</v>
       </c>
       <c r="M152">
         <v>24.08050845850371</v>
@@ -6704,7 +6704,7 @@
         <v>0.222</v>
       </c>
       <c r="L153">
-        <v>5.205962632051441</v>
+        <v>5.205962632051442</v>
       </c>
       <c r="M153">
         <v>34.4895024373408</v>
@@ -6745,10 +6745,10 @@
         <v>0.362</v>
       </c>
       <c r="L154">
-        <v>8.489002129741538</v>
+        <v>8.489002129741539</v>
       </c>
       <c r="M154">
-        <v>56.23963910953768</v>
+        <v>56.2396391095377</v>
       </c>
     </row>
     <row r="155" spans="1:13">
@@ -6786,10 +6786,10 @@
         <v>0.637</v>
       </c>
       <c r="L155">
-        <v>14.93782971448994</v>
+        <v>14.93782971448995</v>
       </c>
       <c r="M155">
-        <v>98.96312185849588</v>
+        <v>98.9631218584959</v>
       </c>
     </row>
     <row r="156" spans="1:13">
@@ -6827,7 +6827,7 @@
         <v>1.073</v>
       </c>
       <c r="L156">
-        <v>25.16215272158196</v>
+        <v>25.16215272158197</v>
       </c>
       <c r="M156">
         <v>166.6992617804805</v>
@@ -6909,10 +6909,10 @@
         <v>3.047</v>
       </c>
       <c r="L158">
-        <v>71.45300963901234</v>
+        <v>71.45300963901235</v>
       </c>
       <c r="M158">
-        <v>473.3761888584567</v>
+        <v>473.3761888584568</v>
       </c>
     </row>
     <row r="159" spans="1:13">
@@ -7032,7 +7032,7 @@
         <v>0.9523333333333334</v>
       </c>
       <c r="L161">
-        <v>22.33248534500145</v>
+        <v>22.33248534500146</v>
       </c>
       <c r="M161">
         <v>147.9527154106346</v>
@@ -7155,7 +7155,7 @@
         <v>0.8170000000000001</v>
       </c>
       <c r="L164">
-        <v>19.15888049723435</v>
+        <v>19.15888049723436</v>
       </c>
       <c r="M164">
         <v>126.9275832941776</v>
@@ -7240,7 +7240,7 @@
         <v>13.92165082234777</v>
       </c>
       <c r="M166">
-        <v>92.23093669805398</v>
+        <v>92.23093669805399</v>
       </c>
     </row>
     <row r="167" spans="1:13">
@@ -7322,7 +7322,7 @@
         <v>8.207598744225246</v>
       </c>
       <c r="M168">
-        <v>54.37534168049225</v>
+        <v>54.37534168049226</v>
       </c>
     </row>
     <row r="169" spans="1:13">
@@ -7360,7 +7360,7 @@
         <v>0.3066666666666667</v>
       </c>
       <c r="L169">
-        <v>7.191419852083071</v>
+        <v>7.191419852083072</v>
       </c>
       <c r="M169">
         <v>47.64315652005035</v>
@@ -7483,7 +7483,7 @@
         <v>0.124</v>
       </c>
       <c r="L172">
-        <v>2.907834983668372</v>
+        <v>2.907834983668373</v>
       </c>
       <c r="M172">
         <v>19.26440676680297</v>
@@ -7524,7 +7524,7 @@
         <v>0.1146666666666667</v>
       </c>
       <c r="L173">
-        <v>2.688965683822366</v>
+        <v>2.688965683822367</v>
       </c>
       <c r="M173">
         <v>17.81439765532318</v>
@@ -7609,7 +7609,7 @@
         <v>1.102163259938819</v>
       </c>
       <c r="M175">
-        <v>7.301831597094672</v>
+        <v>7.301831597094673</v>
       </c>
     </row>
     <row r="176" spans="1:13">
@@ -7688,10 +7688,10 @@
         <v>-0.018</v>
       </c>
       <c r="L177">
-        <v>-0.4221050782744411</v>
+        <v>-0.4221050782744412</v>
       </c>
       <c r="M177">
-        <v>-2.796446143568172</v>
+        <v>-2.796446143568173</v>
       </c>
     </row>
     <row r="178" spans="1:13">
@@ -7729,10 +7729,10 @@
         <v>0.02366666666666667</v>
       </c>
       <c r="L178">
-        <v>0.5549900103238022</v>
+        <v>0.5549900103238024</v>
       </c>
       <c r="M178">
-        <v>3.67680881839519</v>
+        <v>3.676808818395191</v>
       </c>
     </row>
     <row r="179" spans="1:13">
@@ -7814,7 +7814,7 @@
         <v>0.7425922673346651</v>
       </c>
       <c r="M180">
-        <v>4.919673771092156</v>
+        <v>4.919673771092157</v>
       </c>
     </row>
     <row r="181" spans="1:13">
@@ -7852,7 +7852,7 @@
         <v>0.03733333333333334</v>
       </c>
       <c r="L181">
-        <v>0.8754771993840261</v>
+        <v>0.8754771993840263</v>
       </c>
       <c r="M181">
         <v>5.800036445919173</v>
@@ -7937,7 +7937,7 @@
         <v>0.07816760708785947</v>
       </c>
       <c r="M183">
-        <v>0.5178603969570689</v>
+        <v>0.5178603969570691</v>
       </c>
     </row>
     <row r="184" spans="1:13">
@@ -7975,10 +7975,10 @@
         <v>0.019</v>
       </c>
       <c r="L184">
-        <v>0.445555360400799</v>
+        <v>0.4455553604007991</v>
       </c>
       <c r="M184">
-        <v>2.951804262655293</v>
+        <v>2.951804262655294</v>
       </c>
     </row>
     <row r="185" spans="1:13">
@@ -8016,10 +8016,10 @@
         <v>0.024</v>
       </c>
       <c r="L185">
-        <v>0.5628067710325882</v>
+        <v>0.5628067710325884</v>
       </c>
       <c r="M185">
-        <v>3.728594858090897</v>
+        <v>3.728594858090898</v>
       </c>
     </row>
     <row r="186" spans="1:13">
@@ -8098,7 +8098,7 @@
         <v>0.028</v>
       </c>
       <c r="L187">
-        <v>0.6566078995380196</v>
+        <v>0.6566078995380197</v>
       </c>
       <c r="M187">
         <v>4.35002733443938</v>
@@ -8139,10 +8139,10 @@
         <v>0.033</v>
       </c>
       <c r="L188">
-        <v>0.7738593101698088</v>
+        <v>0.7738593101698089</v>
       </c>
       <c r="M188">
-        <v>5.126817929874983</v>
+        <v>5.126817929874984</v>
       </c>
     </row>
     <row r="189" spans="1:13">
@@ -8262,10 +8262,10 @@
         <v>0.024</v>
       </c>
       <c r="L191">
-        <v>0.5628067710325882</v>
+        <v>0.5628067710325884</v>
       </c>
       <c r="M191">
-        <v>3.728594858090897</v>
+        <v>3.728594858090898</v>
       </c>
     </row>
     <row r="192" spans="1:13">
@@ -8303,10 +8303,10 @@
         <v>0.038</v>
       </c>
       <c r="L192">
-        <v>0.8911107208015979</v>
+        <v>0.891110720801598</v>
       </c>
       <c r="M192">
-        <v>5.903608525310586</v>
+        <v>5.903608525310587</v>
       </c>
     </row>
     <row r="193" spans="1:13">
@@ -8344,10 +8344,10 @@
         <v>0.034</v>
       </c>
       <c r="L193">
-        <v>0.7973095922961667</v>
+        <v>0.7973095922961668</v>
       </c>
       <c r="M193">
-        <v>5.282176048962104</v>
+        <v>5.282176048962105</v>
       </c>
     </row>
     <row r="194" spans="1:13">
@@ -8429,7 +8429,7 @@
         <v>-0.445555360400799</v>
       </c>
       <c r="M195">
-        <v>-2.951804262655293</v>
+        <v>-2.951804262655294</v>
       </c>
     </row>
     <row r="196" spans="1:13">
@@ -8508,10 +8508,10 @@
         <v>0.033</v>
       </c>
       <c r="L197">
-        <v>0.7738593101698088</v>
+        <v>0.7738593101698089</v>
       </c>
       <c r="M197">
-        <v>5.126817929874983</v>
+        <v>5.126817929874984</v>
       </c>
     </row>
     <row r="198" spans="1:13">
@@ -8552,7 +8552,7 @@
         <v>1.242864952696966</v>
       </c>
       <c r="M198">
-        <v>8.233980311617396</v>
+        <v>8.233980311617398</v>
       </c>
     </row>
     <row r="199" spans="1:13">
@@ -8590,10 +8590,10 @@
         <v>0.024</v>
       </c>
       <c r="L199">
-        <v>0.5628067710325882</v>
+        <v>0.5628067710325884</v>
       </c>
       <c r="M199">
-        <v>3.728594858090897</v>
+        <v>3.728594858090898</v>
       </c>
     </row>
     <row r="200" spans="1:13">
@@ -8713,10 +8713,10 @@
         <v>0.048</v>
       </c>
       <c r="L202">
-        <v>1.125613542065176</v>
+        <v>1.125613542065177</v>
       </c>
       <c r="M202">
-        <v>7.457189716181794</v>
+        <v>7.457189716181796</v>
       </c>
     </row>
     <row r="203" spans="1:13">
@@ -8757,7 +8757,7 @@
         <v>0.445555360400799</v>
       </c>
       <c r="M203">
-        <v>2.951804262655293</v>
+        <v>2.951804262655294</v>
       </c>
     </row>
     <row r="204" spans="1:13">
@@ -8798,7 +8798,7 @@
         <v>1.219414670570608</v>
       </c>
       <c r="M204">
-        <v>8.078622192530275</v>
+        <v>8.078622192530277</v>
       </c>
     </row>
     <row r="205" spans="1:13">
@@ -8918,7 +8918,7 @@
         <v>0.029</v>
       </c>
       <c r="L207">
-        <v>0.6800581816643775</v>
+        <v>0.6800581816643776</v>
       </c>
       <c r="M207">
         <v>4.505385453526501</v>
@@ -8959,10 +8959,10 @@
         <v>0.024</v>
       </c>
       <c r="L208">
-        <v>0.5628067710325882</v>
+        <v>0.5628067710325884</v>
       </c>
       <c r="M208">
-        <v>3.728594858090897</v>
+        <v>3.728594858090898</v>
       </c>
     </row>
     <row r="209" spans="1:13">
@@ -9044,7 +9044,7 @@
         <v>1.242864952696966</v>
       </c>
       <c r="M210">
-        <v>8.233980311617396</v>
+        <v>8.233980311617398</v>
       </c>
     </row>
     <row r="211" spans="1:13">
@@ -9164,10 +9164,10 @@
         <v>0.024</v>
       </c>
       <c r="L213">
-        <v>0.5628067710325882</v>
+        <v>0.5628067710325884</v>
       </c>
       <c r="M213">
-        <v>3.728594858090897</v>
+        <v>3.728594858090898</v>
       </c>
     </row>
     <row r="214" spans="1:13">
@@ -9246,7 +9246,7 @@
         <v>0.028</v>
       </c>
       <c r="L215">
-        <v>0.6566078995380196</v>
+        <v>0.6566078995380197</v>
       </c>
       <c r="M215">
         <v>4.35002733443938</v>
@@ -9290,7 +9290,7 @@
         <v>0.445555360400799</v>
       </c>
       <c r="M216">
-        <v>2.951804262655293</v>
+        <v>2.951804262655294</v>
       </c>
     </row>
     <row r="217" spans="1:13">
@@ -9413,7 +9413,7 @@
         <v>0.445555360400799</v>
       </c>
       <c r="M219">
-        <v>2.951804262655293</v>
+        <v>2.951804262655294</v>
       </c>
     </row>
     <row r="220" spans="1:13">
@@ -9495,7 +9495,7 @@
         <v>1.219414670570608</v>
       </c>
       <c r="M221">
-        <v>8.078622192530275</v>
+        <v>8.078622192530277</v>
       </c>
     </row>
     <row r="222" spans="1:13">
@@ -9533,10 +9533,10 @@
         <v>0.034</v>
       </c>
       <c r="L222">
-        <v>0.7973095922961667</v>
+        <v>0.7973095922961668</v>
       </c>
       <c r="M222">
-        <v>5.282176048962104</v>
+        <v>5.282176048962105</v>
       </c>
     </row>
     <row r="223" spans="1:13">

</xml_diff>